<commit_message>
update sự phối trong câu
</commit_message>
<xml_diff>
--- a/file/exercise.xlsx
+++ b/file/exercise.xlsx
@@ -2,13 +2,15 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
+  <workbookPr showObjects="none" filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="12 thì" sheetId="1" r:id="rId1"/>
     <sheet name="Sự phối thì" sheetId="6" r:id="rId2"/>
+    <sheet name="Hòa hợp giữa chủ ngữ và động tu" sheetId="7" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId4"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -20,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="681">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1246" uniqueCount="919">
   <si>
     <t>question</t>
   </si>
@@ -2708,12 +2710,899 @@
 – Căn cứ vào đây là mệnh đề trạng ngữ chỉ thời gian: V (nguyên dạng)/Don’t + V (nguyên dạng) + until/As soon as + S + V (hiện tại đơn/ hiện tại hoàn thành).
 – Dịch: Hãy gửi cho chúng tôi bưu thiếp ngay sau khi bạn đến London</t>
   </si>
+  <si>
+    <t>A large number of students in Chu Van An high school_______English fluently.</t>
+  </si>
+  <si>
+    <t>speaks</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is speaking</t>
+  </si>
+  <si>
+    <t>has spoken</t>
+  </si>
+  <si>
+    <t>speak</t>
+  </si>
+  <si>
+    <t>Five billion dollars _____ not enough to aid the victims of the earthquake.</t>
+  </si>
+  <si>
+    <t>were</t>
+  </si>
+  <si>
+    <t>is</t>
+  </si>
+  <si>
+    <t>are</t>
+  </si>
+  <si>
+    <t>A series of lectures _____ being presented at the Central Hall this week.</t>
+  </si>
+  <si>
+    <t>will be</t>
+  </si>
+  <si>
+    <t>has become</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+* Giải thích: A series of + N(số nhiều) + V(số ít).
+* Dịch nghĩa: Một chuỗi bài giảng sẽ được trình bày ở trung tâm hội nghị tuần này.</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+- Cụm danh từ “A number of + N (số nhiều)” thì V (chia số nhiều).
+=&gt; Dùng “large” trước “number” để bổ nghĩa và nhấn mạnh thêm hàm ý muốn nói là “rất nhiều”
+- Dịch nghĩa: Những học sinh ở trường cấp ba Chu Văn An nói tiếng anh rất trôi chảy.</t>
+  </si>
+  <si>
+    <t>Beauty as well as health ___ failed her term</t>
+  </si>
+  <si>
+    <t>have</t>
+  </si>
+  <si>
+    <t>Two years in a strange country ___ like a long time for lonely people.</t>
+  </si>
+  <si>
+    <t>is appearing</t>
+  </si>
+  <si>
+    <t>has appeared</t>
+  </si>
+  <si>
+    <t>appears</t>
+  </si>
+  <si>
+    <t>appeared</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+Trong câu hai danh từ nối với nhau bằng “as well as” nên động từ chia theo chủ ngữ thứ nhất.
+- Chủ ngữ một là “beauty” nên động từ chia số ít. Do đó ta loại B,D
+- Sau động từ “failed” có tân ngữ “her term” nên ta xác định câu này là câu chủ động, không thể chia ở thể bị động
+- Dịch nghĩa: Sức khỏe cũng như sắc đẹp đã làm nhiệm kì này của cô ấy thất bại</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Trong câu chủ ngữ là đại lượng chỉ tiền bạc nên động từ chia số ít. Khi chủ ngữ là đại lượng, đơn vị liên quan đến tiền bạc thì ta luôn chia số ít.
+- Dịch nghĩa: Năm tỷ đô-la thì không đủ để cứu trợ các nạn nhân của trận động đất.</t>
+  </si>
+  <si>
+    <t>-Đáp án C
+- Câu diễn tả một sự thật, một thực tế mà ai cũng thừa nhận như một điều đương nhiên =&gt; chia hiện tại đơn
+=&gt; Trong câu chủ ngữ là đại lượng chỉ thời gian nên động từ chia số ít.
+- Dịch nghĩa: Hai năm ở một đất nước xa lạ dường như quá lâu với những người cô đơn</t>
+  </si>
+  <si>
+    <t>Peter, with his two buddies, ____ the cherry tree now.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> has split</t>
+  </si>
+  <si>
+    <t>have split</t>
+  </si>
+  <si>
+    <t>is splitting</t>
+  </si>
+  <si>
+    <t>are splitting</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Trong câu khi hai danh từ nối với nhau bằng “with” thì động từ chia theo chủ ngữ thứ nhất.
+- Chủ ngữ một là “Peter” nên động từ chia số ít.
+- “Now” là dấu hiệu của thì hiện tại tiếp diễn.
+- Dịch nghĩa: Bây giờ Peter cùng với hai người bạn thân của anh ấy đang chẻ cây anh đào màu đỏ.</t>
+  </si>
+  <si>
+    <t>Bread and butter ___ what Jane asks for.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+- Trong câu hai danh từ nối với nhau bằng“and” nên động từ chia số nhiều. Tuy nhiên nếu hai danh từ nối với nhau bằng “and” mà chỉ cùng một người/một món ăn/một bộ phận thì động từ lại chia số ít.
+- Dịch nghĩa: Bánh mỳ bơ là những gì Jane yêu cầu</t>
+  </si>
+  <si>
+    <t>If anyone ____, tell them I will call when I come back.</t>
+  </si>
+  <si>
+    <t>was calling</t>
+  </si>
+  <si>
+    <t>called</t>
+  </si>
+  <si>
+    <t>call</t>
+  </si>
+  <si>
+    <t>calls</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+- Khi chủ ngữ là “anyone” thì động từ chia số ít.
+- Dịch nghĩa: Nếu ai đó gọi, hãy nói họ tôi sẽ gọi khi tôi quay trở lại.</t>
+  </si>
+  <si>
+    <t>The film “Titanic” __ very interesting and romantic.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+-Khi chủ ngữ là tựa đề của một bộ phim thì động từ chia số ít. Và đó là sự thật hiển nhiên, một đặc điểm, tính chất của sự vật hiện tượng được nhiều người công nhận, nên ta chia hiện tại đơn.
+- Dịch nghĩa: Bộ phim Titanic thì rất thú vị và lãng mạn.</t>
+  </si>
+  <si>
+    <t>Mathematics ___ my favorite subject.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+- Chủ ngữ là danh từ chỉ tên môn học ở dạng số nhiều nhưng theo quy tắc động chia số ít.
+- Dịch nghĩa: Toán là môn học yêu thích của tôi.</t>
+  </si>
+  <si>
+    <t>Neither the parents nor the children _____ aware of the danger.</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Dịch nghĩa: Cả bố mẹ và con cái đều không nhận thức được sự nguy hiểm đó.
+* Cấu trúc:
+- Be aware of st: ý thức về cái gì
+- Neither + S1 + nor + S2 + V(chia theo chủ ngữ 2). Do đó, ta loại B, D vì “children” là danh từ số nhiều
+- Câu này mang ý đưa ra nhận xét nên ta chọn chia ở thì hiện tại đơn</t>
+  </si>
+  <si>
+    <t>The Browns ____ in New York since they migrated to America in 2000.</t>
+  </si>
+  <si>
+    <t>are living</t>
+  </si>
+  <si>
+    <t>have lived</t>
+  </si>
+  <si>
+    <t>have been living</t>
+  </si>
+  <si>
+    <t>has been living</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Chủ ngữ “the Browns” (gia đình nhà Browns) là danh từ số nhiều.
+* Cấu trúc: S + V (hiện tại hoàn thành) since S + V (quá khứ đơn).
+- Dịch nghĩa: Gia đình Brown đã sống ở New York từ khi họ di cư đến Mỹ năm 2000.
+=&gt; Khi muốn nhấn mạnh quá trình của hành động ta dùng thì hiện tại hoàn thành tiếp diễn thay cho thì hiện tại hoàn thành</t>
+  </si>
+  <si>
+    <t>Each of the boys in my class ____ the football team.</t>
+  </si>
+  <si>
+    <t>joins</t>
+  </si>
+  <si>
+    <t>have joined</t>
+  </si>
+  <si>
+    <t>are joining</t>
+  </si>
+  <si>
+    <t>join</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+- Each + of + danh từ/ đại từ số nhiều thì V (chia số ít).
+- Dịch nghĩa: Mỗi cậu bé trong lớp học của tôi tham gia vào đội bóng đá.</t>
+  </si>
+  <si>
+    <t>Neither of the restaurants we went to ____ expensive.</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Neither + of + danh từ/ đại từ số nhiều + V(số ít)
+- Dịch nghĩa: Chẳng nhà hàng nào chúng tôi đến là đắt cả</t>
+  </si>
+  <si>
+    <t>Neither Mary nor her brothers _____ a consent form for tomorrow’s field trip.</t>
+  </si>
+  <si>
+    <t>need</t>
+  </si>
+  <si>
+    <t>needs</t>
+  </si>
+  <si>
+    <t>is needing</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> has needed</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+* Giải thích:
+- Trong câu khi hai chủ ngữ nối với nhau bằng cấu trúc “neither … nor” thì động từ chia theo chủ ngữ hai.
+- Chủ ngữ hai là “her brothers” nên động từ chia số nhiều.</t>
+  </si>
+  <si>
+    <t>Here ___ notebook and report that I promised you last week.</t>
+  </si>
+  <si>
+    <t>is the</t>
+  </si>
+  <si>
+    <t>are the</t>
+  </si>
+  <si>
+    <t>was the</t>
+  </si>
+  <si>
+    <t>were the</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+=&gt; Vì: khi Here đứng đầu câu thì động từ chia theo chủ ngữ đứng sau là the notebook and report. Vì the notebook and report là cùng một vật (cuốn sổ ghi chép và báo cáo) nên động từ chia theo số ít.
+=&gt; Dịch: Đây là cuốn sổ ghi chép và báo cáo mà tôi đã hứa với bạn cuối tuần trước.</t>
+  </si>
+  <si>
+    <t>Mr. John, accompanied by several members of the committee, ____ proposed some changes of the rules.</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+- Trong câu khi hai danh từ nối với nhau bằng “accompanied by” thì động từ chia theo chủ ngữ thứ nhất.
+- Chủ ngữ một “Mr.John” nên động từ chia số ít.
+* Dịch nghĩa: Mr. John cùng với một vài thành viên của hội đồng đã đề xuất một vài thay đổi trong quy định</t>
+  </si>
+  <si>
+    <t>Advertisements on YouTube ____ becoming more competitive than ever before.</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Chủ ngữ “advertisements” là danh từ số nhiều nên V (chia số nhiều).
+- Dịch nghĩa: Những quảng cáo trên YouTube ngày càng trở nên có sức cạnh tranh hơn trước đây.</t>
+  </si>
+  <si>
+    <t>A number of sheep ___ died of a strange illness.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+* Giải thích:
+- Cụm danh từ “A number of “+ N (số nhiều) + V (chia số nhiều). Từ đó, ta loại B, C
+- Do “die” là nội động từ nên không có dạng bị động nên ta loại D
+- Sheep (n): con cừu (vừa là danh từ số ít vừa là danh từ số nhiều)
+* Dịch: Nhiều con cừu đã chết vì bệnh lạ.</t>
+  </si>
+  <si>
+    <t>Half of the letters she sent him ____ in purple ink.</t>
+  </si>
+  <si>
+    <t>wrote</t>
+  </si>
+  <si>
+    <t>has written</t>
+  </si>
+  <si>
+    <t>was written</t>
+  </si>
+  <si>
+    <t>were written</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+- Half + N (số nhiều) thì V (chia số nhiều) vì cấu trúc: “Half of + N + V(chia theo N)”
+- Dịch nghĩa: Một nửa số lá thư cô ấy gửi cho anh ấy đã được viết bằng mực tím.</t>
+  </si>
+  <si>
+    <t>Either Laura or her husband _____ breakfast each morning</t>
+  </si>
+  <si>
+    <t>make</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is making</t>
+  </si>
+  <si>
+    <t>makes</t>
+  </si>
+  <si>
+    <t>made</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+=&gt; Trong câu khi hai danh từ nối với nhau bằng cấu trúc “either … or” thì động từ chia theo chủ
+ngữ hai.
+- Chủ ngữ hai là “her husband” nên động từ chia số ít.
+* Dịch nghĩa: Hoặc Laura hoặc chồng cô ấy làm bữa sáng.</t>
+  </si>
+  <si>
+    <t>The army ____ eliminated this section of the training test</t>
+  </si>
+  <si>
+    <t>is having</t>
+  </si>
+  <si>
+    <t>What he told you ___ to be of no importance.</t>
+  </si>
+  <si>
+    <t>seems</t>
+  </si>
+  <si>
+    <t>seem</t>
+  </si>
+  <si>
+    <t>must seem</t>
+  </si>
+  <si>
+    <t>have seemed</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+*Theo cấu trúc mệnh đề danh từ: That/wh_/…+ S + V1(chia theo S) + V(chính, luôn chia ở dạng số ít)+…..
+=&gt; Do đó, động từ cần chia chỉ có thể là A hoặc C. Xét nghĩa ta chọn A
+* Dịch: Điều anh ta đã nói với bạn dường như là không quan trọng</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+- Căn cứ vào danh từ army (quân đội) là danh từ chỉ tập hợp nên động từ chia ở dạng số nhiều.
+* Ta loại phương án A và B. Đây là một quy tắc cần ghi nhớ trong sự hòa hợp giữa chủ ngữ và động từ. Ta hiểu rằng “quân đội” ở đây ám chỉ những người/cán bộ trong quân đội nên nó sẽ mang tính chất số nhiều -&gt; động từ chia số nhiều.
+- Căn cứ vào nghĩa của câu: Quân đội đã loại bỏ phần này trong bài kiểm tra huấn luyện.
+=&gt; Câu mang nghĩa chủ động nên ta loại phương án C.</t>
+  </si>
+  <si>
+    <t>Psychologists have found that the number of social contacts we have _____ only reason for loneliness.</t>
+  </si>
+  <si>
+    <t>are not the</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> is not the</t>
+  </si>
+  <si>
+    <t>are not an</t>
+  </si>
+  <si>
+    <t>is not an</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+- Cụm danh từ “The number of” + N (số nhiều) thì V (chia số ít): số lượng cái gì….
+- Ta dùng cụm từ: “the only + N: cái gì duy nhất”, do đó chọn B
+* Dịch nghĩa: Những nhà tâm lí học đã phát hiện ra rằng số lượng những mối quan hệ xã hội mà chúng ta có không phải là lí do duy nhất cho sự cô đơn.</t>
+  </si>
+  <si>
+    <t>The flock of birds_____ circling overhead.</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Khi hai danh từ nối với nhau bằng “of” thì động từ chia theo chủ ngữ thứ nhất.
+- Chủ ngữ một là “the flock”-bầy/đàn như một thể thống nhất, không phải riêng biệt dù chúng bao gồm nhiêu con trong đó, nên động từ chia số ít.
+*Dịch nghĩa: Đàn chim đang bay vòng tròn trên bầu trời.</t>
+  </si>
+  <si>
+    <t>The use of credit cards in place of cash ______ increased rapidly in recently years.</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+* Căn cứ: Khi hai danh từ nối với nhau bằng “of” thì động từ chia theo chủ ngữ thứ nhất.
+* Chủ ngữ một là “the use” là số ít, ở đây đơn thuần mang nghĩa chủ động vì “việc sử dụng đó” tự nó tăng lên do nhu cầu sử dụng nhiều của con người chứ không phải con người cố ý làm cho nó tăng lên
+* Dịch nghĩa: Việc sử dụng những chiếc thẻ tín dụng thay thế tiền mặt đã tăng lên nhanh chóng trong những năm gần đây.</t>
+  </si>
+  <si>
+    <t>The fact that the new staff members were complimented on their achievement ____ known to the whole company</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Trong mệnh đề quan hệ động từ chia theo danh từ ở mệnh đề chính là “the fact”. Vì câu đã có mệnh đề quan hệ “that the new….their achievement” nên vị trí còn thiếu phải là động từ chính của câu.
+=&gt; Danh từ “the fact” nên động từ chia số ít. Động từ cần chia bị động “được biết đến” nên còn thiếu “tobe” -&gt; chia “was”
+* Dịch nghĩa: Thực tế rằng việc toàn thể nhân viên mới đã được khen ngợi vì thành tích của họ đã
+được biết đến trong toàn bộ công ty.</t>
+  </si>
+  <si>
+    <t>If nobody ___ bought that car from the dealer, then you should return and make another offer.</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+=&gt; Key: D. has
+=&gt; Vì: khi chủ ngữ là đại từ bất định như nobody thì động từ chia số ít và không dùng thì tương lai trong mệnh đề If
+=&gt; Dịch: Nếu không có ai mua chiếc xe đó từ đại lý, thì bạn nên quay lại và đưa ra một đề nghị khác.</t>
+  </si>
+  <si>
+    <t>Massachusetts and Connecticut ___ located in New England.</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+=&gt; Vì: chủ ngữ là số nhiều và diễn tả sự thật hiển nhiên
+* Dịch: Massachusetts and Connecticut nằm ở New England</t>
+  </si>
+  <si>
+    <t>Everything ___ bright and clean.</t>
+  </si>
+  <si>
+    <t>looking</t>
+  </si>
+  <si>
+    <t>to look</t>
+  </si>
+  <si>
+    <t>looks</t>
+  </si>
+  <si>
+    <t>is looking</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Vì đại từ bất định “everything” đi với động từ số ít. Loại đáp án D vì động từ tri giác “look” khi mang nghĩa “trông ra làm sao” thì nó không bao giờ dùng ở dạng tiếp diễn.
+*Dịch: Mọi thứ trông sáng sủa và sạch sẽ.</t>
+  </si>
+  <si>
+    <t>Much homework ___ given to students every day</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+=&gt; Vì: Homework là danh từ không đếm được. Ta dùng: Much + N(không đếm được) + V(số ít):
+nhiều cái gì. Hơn nữa, có everyday nên ta chia thì hiện tại đơn
+* Dịch: Nhiều bài tập về nhà được giao cho học sinh mỗi ngày</t>
+  </si>
+  <si>
+    <t>The facilities at the new research library, including an excellent microfilm file,____ wonderful.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+=&gt; Vì: động từ chia theo chủ ngữ “facilities”, là danh từ số nhiều =&gt; động từ ở dạng số nhiều
+*Dịch: Cơ sở vật chất tại thư viện nghiên cứu mới, bao gồm một tệp vi phim thì tuyệt vời</t>
+  </si>
+  <si>
+    <t>The police ___ making enquiries about the murder.</t>
+  </si>
+  <si>
+    <t>be</t>
+  </si>
+  <si>
+    <t>To do such a hard work___ so many people.</t>
+  </si>
+  <si>
+    <t>needing</t>
+  </si>
+  <si>
+    <t>to need</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+=&gt; Key: D. needs
+=&gt; Vì: khi chủ ngữ là cụm To + V thì động từ theo sau phải chia ở dạng số it
+*Dịch: Để thực hiện một công việc khó cần rất nhiều người</t>
+  </si>
+  <si>
+    <t>The methods for studying the world _____ been developed slowly through the work of many people.</t>
+  </si>
+  <si>
+    <t>having</t>
+  </si>
+  <si>
+    <t>to have</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+=&gt; Vì: Chủ ngữ là “The methods for studying the world” =&gt; Danh từ số nhiều =&gt; động từ chia ở dạng số nhiều
+* Dịch: Các phương pháp nghiên cứu thế giới được phát triển chậm thông qua công việc của nhiều người.</t>
+  </si>
+  <si>
+    <t>The regulations governing animal research ___ many provisions to safeguard animal welfare.</t>
+  </si>
+  <si>
+    <t>contains</t>
+  </si>
+  <si>
+    <t>contain</t>
+  </si>
+  <si>
+    <t>have been contained</t>
+  </si>
+  <si>
+    <t>is containing</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+=&gt; Key: B. contain
+=&gt; Vì: câu mang nghĩa là một sự thật hiển nhiên, chia hiện tại đơn; với chủ ngữ là “The regulations governing animal research”, danh từ số nhiều =&gt; động từ chia số nhiều
+* Dịch: Các quy định quản lý nghiên cứu động vật bao gồm nhiều quy định để bảo vệ sức khỏe động vật.</t>
+  </si>
+  <si>
+    <t>Thanks to the recent anti-smoking campaign, the number of smokers in the country ___.</t>
+  </si>
+  <si>
+    <t>has reduced</t>
+  </si>
+  <si>
+    <t>reduce</t>
+  </si>
+  <si>
+    <t>to reduce</t>
+  </si>
+  <si>
+    <t>having reduced</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+- Vì: the number of + N + V chia số ít: số lượng ai/cái gì….
+*Dịch: Nhờ chiến dịch chống hút thuốc gần đây, số người hút thuốc trong nước đã giảm</t>
+  </si>
+  <si>
+    <t>Each of the 4 types of human ___ suited for a specific purpose.</t>
+  </si>
+  <si>
+    <t>tooth are</t>
+  </si>
+  <si>
+    <t>teeth is</t>
+  </si>
+  <si>
+    <t>tooth is</t>
+  </si>
+  <si>
+    <t>teeth are</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+=&gt; Vì: rằng người là sô nhiều =&gt; dùng teeth, nguyên tắc each of + N số nhiều + V số ít =&gt; chọn teeth is
+*Dịch: Mỗi loại trong số 4 loại răng của con người đều phù hợp cho một mục đích cụ thể</t>
+  </si>
+  <si>
+    <t>There ____ shops on either side of the street many years ago.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+=&gt; Key: A. were
+=&gt; Vì: khi câu bắt đầu bằng There thì động từ chia theo danh từ phía sau, ở đây shops là danh từ
+số nhiều =&gt; động từ ở dạng số nhiều, có dấu hiệu nhận biết củ thì quá khứ đơn ago =&gt; were
+*Dịch: Đã từng có nhiều cửa hàng ở hai bên đường nhiều năm trước</t>
+  </si>
+  <si>
+    <t>Neither of my parents ____my boyfriend.</t>
+  </si>
+  <si>
+    <t>like</t>
+  </si>
+  <si>
+    <t>likes</t>
+  </si>
+  <si>
+    <t>liked</t>
+  </si>
+  <si>
+    <t>has liked</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+- Neither + of + danh từ/ đại từ số nhiều + V(số ít)
+*Dịch nghĩa: Cả hai bố mẹ tôi đều không thích bạn trai tôi.</t>
+  </si>
+  <si>
+    <t>The teams ______ends at half-time so that neither side has an unfair advantage.</t>
+  </si>
+  <si>
+    <t>has changed</t>
+  </si>
+  <si>
+    <t>change</t>
+  </si>
+  <si>
+    <t>changes</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+=&gt; Key: B. change
+=&gt; Vì: động từ sau teams chia ở dạng số nhiều và ở đây là thì hiện tại đơn =&gt; change
+*Dịch: Các đội thay đổi kết thúc ở một nửa thời gian để không bên nào có lợi thế không công bằng</t>
+  </si>
+  <si>
+    <t>Physics ____ my favorite subject when I was at high school.</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Physics (môn vật lý) mặc dù tận cùng bằng -s nhưng chỉ tên một môn học -&gt; danh từ số ít.
+- Do đó, động từ cần chia ở dạng số ít. Ta loại phương án B và D.
+*Dịch nghĩa: Môn vật lý là môn học yêu thích của tôi khi còn học phổ thông.
+=&gt; Do có mệnh đề trạng ngữ chỉ thời gian (when I was at high school) nên động từ trong mệnh đề chính chia thì quá khứ đơn.</t>
+  </si>
+  <si>
+    <t>The unemployed ___ to live on the unemployment benefits</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+* Vì:
+- The unemployed (những người thất nghiệp) + động từ ở dạng số nhiều
+- Ở đây diễn tả sự việc diễn ra thường xuyên =&gt; hiện tại đơn
+*Note: “The + adj”: chỉ tập thể những người có đặc điểm, tính chất adj đó.
+*Dịch: Những người thất nghiệp phải sống dựa vào khoản trợ cấp thất nghiệp</t>
+  </si>
+  <si>
+    <t>Why he was absent from the class yesterday ___ unknown.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+- Căn cứ: chủ ngữ là mệnh đề danh từ: “why + S + V” =&gt; Động từ “to be” chia số ít =&gt; chia “is”.
+*Dịch nghĩa: Việc tại sao anh ấy vắng mặt ở lớp ngày hôm qua thì không được biết đến.</t>
+  </si>
+  <si>
+    <t>I’m poor! Nobody ____ me.” “I know a person who ____ you. It’s me.”</t>
+  </si>
+  <si>
+    <t>love/likes</t>
+  </si>
+  <si>
+    <t>loves/like</t>
+  </si>
+  <si>
+    <t>loves/likes</t>
+  </si>
+  <si>
+    <t>love/like</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+=&gt; Key: C. loves/likes
+=&gt; Vì: chỗ trống đầu tiên: động từ sau Nobody phải chia ở dạng số ít, chỗ trống thứ 2 thì động từ có chủ ngữ là a person =&gt; chia ở dạng số ít
+*Dịch: “Tôi rất đáng thương. Không ai yêu thích tôi cả “. “ Tôi biết một người thích bạn. Đó là tôi”</t>
+  </si>
+  <si>
+    <t>The furniture he has in his bedroom ____ a bed and a table</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+=&gt; Key: A. is
+=&gt; Vì: Furniture là danh từ không đếm được =&gt; động từ chia ở dạng số ít, câu này ở hiện tại đơn =&gt; is
+* Dịch: Nội thất anh ta có trong phòng ngủ của anh ta là một cái giường và một cái bàn.</t>
+  </si>
+  <si>
+    <t>Learning English to find a better job ____ my aim in the next time.</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+=&gt; Key: A. is
+=&gt; Vì: chủ ngữ là learning english =&gt; chia động từ số ít, do đang diễn tả mục đích hiện tại =&gt; hiện tại đơn
+* Dịch: Việc học tiếng anh để tìm một công việc tốt hơn là mục tiêu của tôi trong thời gian tới</t>
+  </si>
+  <si>
+    <t>Can I borrow your dictionary for a moment? Mine ____</t>
+  </si>
+  <si>
+    <t>have been lef</t>
+  </si>
+  <si>
+    <t>has been lef</t>
+  </si>
+  <si>
+    <t>was left</t>
+  </si>
+  <si>
+    <t>were left</t>
+  </si>
+  <si>
+    <t>- Đáp án B
+=&gt; Key: B. has been left
+=&gt; Vì: Mine là cái của tôi =&gt; danh từ số ít =&gt; động từ chia số ít, mà ở đây diễn tả việc bỏ quên từ điển ở 1 thời điểm không xác định trong quá khứ =&gt; dùng thì hiện tại hoàn thành
+* Dịch: Tôi có thể mượn từ điển của bạn một lúc không? Quyển của tôi đã bị để quên rồi</t>
+  </si>
+  <si>
+    <t>According to the announcement, only 30% of the applicants _____selected for the next interview.</t>
+  </si>
+  <si>
+    <t>been</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+=&gt; Key: A. are
+=&gt; Vì: chủ ngữ là 30% =&gt; dựa vào danh từ sau of để chia, applicants là danh từ số nhiều =&gt; động từ chia ở dạng sso nhiều
+* Dịch: Theo thông báo, chỉ có 30% số người nộp đơn được chọn cho cuộc phỏng vấn tiếp theo</t>
+  </si>
+  <si>
+    <t>The development of popular music through the ages _____by the documentary.</t>
+  </si>
+  <si>
+    <t>was traced</t>
+  </si>
+  <si>
+    <t xml:space="preserve">were traced </t>
+  </si>
+  <si>
+    <t>have been traced</t>
+  </si>
+  <si>
+    <t>are traced</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+- Trong câu khi hai danh từ nối với nhau bằng “of” thì động từ chia theo danh từ thứ nhất.
+- Danh từ “the development” nên động từ chia số ít.
+* Dịch nghĩa: Sự phát triển phổ biến của âm nhạc qua nhiều năm đã được đánh dấu bằng phim tài liệu.</t>
+  </si>
+  <si>
+    <t>Living expenses in this country, as well as in many others, is at an all-time high.</t>
+  </si>
+  <si>
+    <t>Living</t>
+  </si>
+  <si>
+    <t>as well as</t>
+  </si>
+  <si>
+    <t>all-time</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Trong câu hai danh từ nối với nhau bằng “as well as” nên động từ chia theo chủ ngữ thứ nhất.
+- Chủ ngữ một “Living expenses” là danh từ số nhiều nên động từ phải chia ở dạng số nhiều (is =&gt; are)
+*Dịch nghĩa: Chi phí sinh hoạt ở vùng này cũng như nhiều nơi khác ở mức cao chưa từng thấy</t>
+  </si>
+  <si>
+    <t>The effects of cigarette smoking has been proven to be extremely harmful.</t>
+  </si>
+  <si>
+    <t>The</t>
+  </si>
+  <si>
+    <t>cigarette smoking</t>
+  </si>
+  <si>
+    <t>extremely</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Đáp án: has =&gt; have
+*Giải thích:
+- Trong câu hai danh từ nối với nhau bằng “of” thì động từ chia theo chủ ngữ thứ nhất.
+- Chủ ngữ một là “the effects” nên động từ chia số nhiều.
+*Dịch nghĩa: Những ảnh hưởng của việc hút thuốc lá đã được chứng minh cực kì có hại</t>
+  </si>
+  <si>
+    <t>It is impossible to believe that somebody actually admire that man.</t>
+  </si>
+  <si>
+    <t>impossible</t>
+  </si>
+  <si>
+    <t>believe</t>
+  </si>
+  <si>
+    <t>actually</t>
+  </si>
+  <si>
+    <t>admire</t>
+  </si>
+  <si>
+    <t>- Đáp án D
+- admire =&gt; admires
+- Khi chủ ngữ là đại từ bất định như: someone, anyone,… thì động từ chia số ít.
+- Trong câu chủ ngữ là “somebody”.
+*Dịch nghĩa: Không thể tin rằng mọi người thực sự ngưỡng mộ người đàn ông đó.</t>
+  </si>
+  <si>
+    <t>Every Elementary School teacher have to take a training course.</t>
+  </si>
+  <si>
+    <t>Every</t>
+  </si>
+  <si>
+    <t>Elementary</t>
+  </si>
+  <si>
+    <t>have to</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- have =&gt; has to
+- Khi chủ ngữ bắt đầu bằng “every” thì động từ chia số ít.
+- Chủ ngữ của câu “Every Elementary School teacher”.
+*Dịch nghĩa: Mỗi giáo viên ở trường tiểu học phải tham gia một khóa học đào tạo</t>
+  </si>
+  <si>
+    <t>John, along with twenty friends, are celebrating a party.</t>
+  </si>
+  <si>
+    <t>along with</t>
+  </si>
+  <si>
+    <t>friends</t>
+  </si>
+  <si>
+    <t>a party</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- Đáp án: C (are =&gt; is)
+- Trong câu hai danh từ nối với nhau bằng “along with” thì động từ chia theo chủ ngữ thứ nhất.
+- Chủ ngữ một là “John” nên động từ chia số ít.
+*Dịch nghĩa: John cùng với 20 người bạn của anh ấy đang tổ chức một bữa tiệc.</t>
+  </si>
+  <si>
+    <t>Linguistics bring us to further understanding of cultures, societies and civilizations.</t>
+  </si>
+  <si>
+    <t>bring</t>
+  </si>
+  <si>
+    <t>further</t>
+  </si>
+  <si>
+    <t>of</t>
+  </si>
+  <si>
+    <t>societies</t>
+  </si>
+  <si>
+    <t>- Đáp án A
+-bring =&gt; brings
+- Chủ ngữ là “Linguistics” là danh từ đặc biệt chỉ tên môn học (ở dạng số nhiều) nhưng động từ chia số ít.
+*Dịch nghĩa: Ngôn ngữ học mang đến cho chúng ta nhiều hơn hiểu biết về văn hóa, xã hội và những nên văn minh.</t>
+  </si>
+  <si>
+    <t>English is one of the most popular language in the world.</t>
+  </si>
+  <si>
+    <t>most</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>the</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- languge =&gt; languages
+- Ta có “one of + Danh từ số nhiều”: một trong những.
+*Dịch nghĩa: Tiếng anh là một trong những ngôn ngữ phổ biến nhất trên thế giới.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> It is disconcerting to believe that every possible candidate have been rejected for
+one reason or another.</t>
+  </si>
+  <si>
+    <t>disconcerting</t>
+  </si>
+  <si>
+    <t>possible</t>
+  </si>
+  <si>
+    <t>one</t>
+  </si>
+  <si>
+    <t>- Đáp án C
+- have =&gt; has
+- Khi chủ ngữ bắt đầu bằng “every” thì động từ chia số ít.
+- Chủ ngữ của câu “every possible candidate”.
+* Dịch nghĩa: Thật bối rối để tin rằng mỗi ứng viên có thể đã bị từ chối vì lí do này hoặc lí do khác.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2742,6 +3631,12 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -2763,7 +3658,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -2813,6 +3708,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5582,8 +6489,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="G17" sqref="G14:G17"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection sqref="A1:G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5854,4 +6761,1447 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G59"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="F56" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="91.5703125" style="16" customWidth="1"/>
+    <col min="2" max="2" width="14.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" style="19" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" style="19" customWidth="1"/>
+    <col min="5" max="5" width="15.5703125" style="19" customWidth="1"/>
+    <col min="6" max="6" width="9.140625" style="19"/>
+    <col min="7" max="7" width="111.42578125" style="16" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A2" s="16" t="s">
+        <v>681</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>682</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>683</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>684</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>685</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>694</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A3" s="16" t="s">
+        <v>686</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="D3" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="E3" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="F3" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>703</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
+        <v>690</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="C4" s="19" t="s">
+        <v>691</v>
+      </c>
+      <c r="D4" s="19" t="s">
+        <v>692</v>
+      </c>
+      <c r="E4" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="F4" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A5" s="21" t="s">
+        <v>695</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="D5" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="E5" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A6" s="16" t="s">
+        <v>697</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>698</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>699</v>
+      </c>
+      <c r="D6" s="19" t="s">
+        <v>700</v>
+      </c>
+      <c r="E6" s="19" t="s">
+        <v>701</v>
+      </c>
+      <c r="F6" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A7" s="21" t="s">
+        <v>705</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>706</v>
+      </c>
+      <c r="C7" s="19" t="s">
+        <v>707</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>708</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>709</v>
+      </c>
+      <c r="F7" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8" s="16" t="s">
+        <v>711</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C8" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D8" s="19" t="s">
+        <v>691</v>
+      </c>
+      <c r="E8" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="F8" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" s="21" t="s">
+        <v>713</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>714</v>
+      </c>
+      <c r="C9" s="19" t="s">
+        <v>715</v>
+      </c>
+      <c r="D9" s="19" t="s">
+        <v>716</v>
+      </c>
+      <c r="E9" s="19" t="s">
+        <v>717</v>
+      </c>
+      <c r="F9" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10" s="16" t="s">
+        <v>719</v>
+      </c>
+      <c r="B10" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C10" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D10" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="E10" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="F10" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>720</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A11" s="21" t="s">
+        <v>721</v>
+      </c>
+      <c r="B11" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C11" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D11" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E11" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="F11" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>722</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A12" s="16" t="s">
+        <v>723</v>
+      </c>
+      <c r="B12" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="C12" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="D12" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="E12" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F12" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A13" s="21" t="s">
+        <v>725</v>
+      </c>
+      <c r="B13" s="19" t="s">
+        <v>726</v>
+      </c>
+      <c r="C13" s="19" t="s">
+        <v>727</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>728</v>
+      </c>
+      <c r="E13" s="19" t="s">
+        <v>729</v>
+      </c>
+      <c r="F13" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A14" s="16" t="s">
+        <v>731</v>
+      </c>
+      <c r="B14" s="19" t="s">
+        <v>732</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>733</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>734</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>735</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>736</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15" s="21" t="s">
+        <v>737</v>
+      </c>
+      <c r="B15" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="E15" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="F15" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>738</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A16" s="16" t="s">
+        <v>739</v>
+      </c>
+      <c r="B16" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="C16" s="19" t="s">
+        <v>741</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>742</v>
+      </c>
+      <c r="E16" s="19" t="s">
+        <v>743</v>
+      </c>
+      <c r="F16" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A17" s="21" t="s">
+        <v>745</v>
+      </c>
+      <c r="B17" s="19" t="s">
+        <v>746</v>
+      </c>
+      <c r="C17" s="19" t="s">
+        <v>747</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>748</v>
+      </c>
+      <c r="E17" s="19" t="s">
+        <v>749</v>
+      </c>
+      <c r="F17" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>750</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A18" s="16" t="s">
+        <v>751</v>
+      </c>
+      <c r="B18" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="C18" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D18" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="F18" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>752</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19" s="21" t="s">
+        <v>753</v>
+      </c>
+      <c r="B19" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C19" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="D19" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="F19" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>754</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A20" s="16" t="s">
+        <v>755</v>
+      </c>
+      <c r="B20" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="21" t="s">
+        <v>757</v>
+      </c>
+      <c r="B21" s="19" t="s">
+        <v>758</v>
+      </c>
+      <c r="C21" s="19" t="s">
+        <v>759</v>
+      </c>
+      <c r="D21" s="19" t="s">
+        <v>760</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>761</v>
+      </c>
+      <c r="F21" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>762</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A22" s="16" t="s">
+        <v>763</v>
+      </c>
+      <c r="B22" s="19" t="s">
+        <v>764</v>
+      </c>
+      <c r="C22" s="19" t="s">
+        <v>765</v>
+      </c>
+      <c r="D22" s="19" t="s">
+        <v>766</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>767</v>
+      </c>
+      <c r="F22" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>768</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A23" s="21" t="s">
+        <v>769</v>
+      </c>
+      <c r="B23" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C23" s="19" t="s">
+        <v>770</v>
+      </c>
+      <c r="D23" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="F23" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>777</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A24" s="16" t="s">
+        <v>771</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>772</v>
+      </c>
+      <c r="C24" s="19" t="s">
+        <v>773</v>
+      </c>
+      <c r="D24" s="19" t="s">
+        <v>774</v>
+      </c>
+      <c r="E24" s="11" t="s">
+        <v>775</v>
+      </c>
+      <c r="F24" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>776</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A25" s="21" t="s">
+        <v>778</v>
+      </c>
+      <c r="B25" s="19" t="s">
+        <v>779</v>
+      </c>
+      <c r="C25" s="19" t="s">
+        <v>780</v>
+      </c>
+      <c r="D25" s="19" t="s">
+        <v>781</v>
+      </c>
+      <c r="E25" s="11" t="s">
+        <v>782</v>
+      </c>
+      <c r="F25" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A26" s="16" t="s">
+        <v>784</v>
+      </c>
+      <c r="B26" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="C26" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D26" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="E26" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="F26" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>785</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A27" s="21" t="s">
+        <v>786</v>
+      </c>
+      <c r="B27" s="19" t="s">
+        <v>526</v>
+      </c>
+      <c r="C27" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="D27" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="E27" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>787</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A28" s="1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B28" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C28" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="D28" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="E28" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="F28" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>789</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A29" s="16" t="s">
+        <v>790</v>
+      </c>
+      <c r="B29" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="C29" s="19" t="s">
+        <v>230</v>
+      </c>
+      <c r="D29" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="E29" s="11" t="s">
+        <v>228</v>
+      </c>
+      <c r="F29" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>791</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A30" s="21" t="s">
+        <v>792</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="D30" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="E30" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="F30" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>793</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A31" s="16" t="s">
+        <v>794</v>
+      </c>
+      <c r="B31" s="19" t="s">
+        <v>795</v>
+      </c>
+      <c r="C31" s="19" t="s">
+        <v>796</v>
+      </c>
+      <c r="D31" s="19" t="s">
+        <v>797</v>
+      </c>
+      <c r="E31" s="11" t="s">
+        <v>798</v>
+      </c>
+      <c r="F31" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>799</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A32" s="16" t="s">
+        <v>800</v>
+      </c>
+      <c r="B32" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="C32" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="D32" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="E32" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="F32" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>801</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>802</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="C33" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="D33" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="F33" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A34" s="16" t="s">
+        <v>804</v>
+      </c>
+      <c r="B34" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="E34" s="11" t="s">
+        <v>805</v>
+      </c>
+      <c r="F34" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>803</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A35" s="16" t="s">
+        <v>806</v>
+      </c>
+      <c r="B35" s="19" t="s">
+        <v>740</v>
+      </c>
+      <c r="C35" s="19" t="s">
+        <v>807</v>
+      </c>
+      <c r="D35" s="19" t="s">
+        <v>808</v>
+      </c>
+      <c r="E35" s="11" t="s">
+        <v>741</v>
+      </c>
+      <c r="F35" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>809</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A36" s="16" t="s">
+        <v>810</v>
+      </c>
+      <c r="B36" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="C36" s="19" t="s">
+        <v>811</v>
+      </c>
+      <c r="D36" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="E36" s="11" t="s">
+        <v>812</v>
+      </c>
+      <c r="F36" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>813</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A37" s="16" t="s">
+        <v>814</v>
+      </c>
+      <c r="B37" s="19" t="s">
+        <v>815</v>
+      </c>
+      <c r="C37" s="19" t="s">
+        <v>816</v>
+      </c>
+      <c r="D37" s="19" t="s">
+        <v>817</v>
+      </c>
+      <c r="E37" s="11" t="s">
+        <v>818</v>
+      </c>
+      <c r="F37" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>819</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A38" s="16" t="s">
+        <v>820</v>
+      </c>
+      <c r="B38" s="19" t="s">
+        <v>821</v>
+      </c>
+      <c r="C38" s="19" t="s">
+        <v>822</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>823</v>
+      </c>
+      <c r="E38" s="11" t="s">
+        <v>824</v>
+      </c>
+      <c r="F38" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>825</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>826</v>
+      </c>
+      <c r="B39" s="19" t="s">
+        <v>827</v>
+      </c>
+      <c r="C39" s="19" t="s">
+        <v>828</v>
+      </c>
+      <c r="D39" s="11" t="s">
+        <v>829</v>
+      </c>
+      <c r="E39" s="11" t="s">
+        <v>830</v>
+      </c>
+      <c r="F39" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>831</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A40" s="16" t="s">
+        <v>832</v>
+      </c>
+      <c r="B40" s="19" t="s">
+        <v>687</v>
+      </c>
+      <c r="C40" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="E40" s="11" t="s">
+        <v>689</v>
+      </c>
+      <c r="F40" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>833</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A41" s="16" t="s">
+        <v>834</v>
+      </c>
+      <c r="B41" s="19" t="s">
+        <v>835</v>
+      </c>
+      <c r="C41" s="19" t="s">
+        <v>836</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>837</v>
+      </c>
+      <c r="E41" s="11" t="s">
+        <v>838</v>
+      </c>
+      <c r="F41" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>839</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A42" s="16" t="s">
+        <v>840</v>
+      </c>
+      <c r="B42" s="19" t="s">
+        <v>841</v>
+      </c>
+      <c r="C42" s="19" t="s">
+        <v>842</v>
+      </c>
+      <c r="D42" s="19" t="s">
+        <v>843</v>
+      </c>
+      <c r="E42" s="11" t="s">
+        <v>843</v>
+      </c>
+      <c r="F42" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>844</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A43" s="16" t="s">
+        <v>845</v>
+      </c>
+      <c r="B43" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C43" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D43" s="19" t="s">
+        <v>527</v>
+      </c>
+      <c r="E43" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="F43" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>846</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A44" s="16" t="s">
+        <v>847</v>
+      </c>
+      <c r="B44" s="19" t="s">
+        <v>228</v>
+      </c>
+      <c r="C44" s="19" t="s">
+        <v>696</v>
+      </c>
+      <c r="D44" s="19" t="s">
+        <v>231</v>
+      </c>
+      <c r="E44" s="11" t="s">
+        <v>689</v>
+      </c>
+      <c r="F44" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>848</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45" s="21" t="s">
+        <v>849</v>
+      </c>
+      <c r="B45" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C45" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D45" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="E45" s="11" t="s">
+        <v>687</v>
+      </c>
+      <c r="F45" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>850</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A46" s="16" t="s">
+        <v>851</v>
+      </c>
+      <c r="B46" s="19" t="s">
+        <v>852</v>
+      </c>
+      <c r="C46" s="19" t="s">
+        <v>853</v>
+      </c>
+      <c r="D46" s="19" t="s">
+        <v>854</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>855</v>
+      </c>
+      <c r="F46" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>856</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="16" t="s">
+        <v>857</v>
+      </c>
+      <c r="B47" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C47" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="E47" s="11" t="s">
+        <v>526</v>
+      </c>
+      <c r="F47" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>858</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A48" s="16" t="s">
+        <v>859</v>
+      </c>
+      <c r="B48" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C48" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="D48" s="11" t="s">
+        <v>691</v>
+      </c>
+      <c r="E48" s="11" t="s">
+        <v>241</v>
+      </c>
+      <c r="F48" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>860</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A49" s="16" t="s">
+        <v>861</v>
+      </c>
+      <c r="B49" s="19" t="s">
+        <v>862</v>
+      </c>
+      <c r="C49" s="11" t="s">
+        <v>863</v>
+      </c>
+      <c r="D49" s="11" t="s">
+        <v>864</v>
+      </c>
+      <c r="E49" s="11" t="s">
+        <v>865</v>
+      </c>
+      <c r="F49" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>866</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A50" s="16" t="s">
+        <v>867</v>
+      </c>
+      <c r="B50" s="19" t="s">
+        <v>689</v>
+      </c>
+      <c r="C50" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="D50" s="11" t="s">
+        <v>527</v>
+      </c>
+      <c r="E50" s="11" t="s">
+        <v>868</v>
+      </c>
+      <c r="F50" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>869</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A51" s="16" t="s">
+        <v>870</v>
+      </c>
+      <c r="B51" s="11" t="s">
+        <v>871</v>
+      </c>
+      <c r="C51" s="11" t="s">
+        <v>872</v>
+      </c>
+      <c r="D51" s="11" t="s">
+        <v>873</v>
+      </c>
+      <c r="E51" s="11" t="s">
+        <v>874</v>
+      </c>
+      <c r="F51" s="11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>875</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="5" t="s">
+        <v>876</v>
+      </c>
+      <c r="B52" s="17" t="s">
+        <v>877</v>
+      </c>
+      <c r="C52" s="17" t="s">
+        <v>878</v>
+      </c>
+      <c r="D52" s="17" t="s">
+        <v>688</v>
+      </c>
+      <c r="E52" s="17" t="s">
+        <v>879</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>880</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>881</v>
+      </c>
+      <c r="B53" s="19" t="s">
+        <v>882</v>
+      </c>
+      <c r="C53" s="17" t="s">
+        <v>883</v>
+      </c>
+      <c r="D53" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="E53" s="17" t="s">
+        <v>884</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>885</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A54" s="5" t="s">
+        <v>886</v>
+      </c>
+      <c r="B54" s="19" t="s">
+        <v>887</v>
+      </c>
+      <c r="C54" s="17" t="s">
+        <v>888</v>
+      </c>
+      <c r="D54" s="17" t="s">
+        <v>889</v>
+      </c>
+      <c r="E54" s="17" t="s">
+        <v>890</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>891</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A55" s="5" t="s">
+        <v>892</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>893</v>
+      </c>
+      <c r="C55" s="5" t="s">
+        <v>894</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>895</v>
+      </c>
+      <c r="E55" s="19" t="s">
+        <v>896</v>
+      </c>
+      <c r="F55" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G55" s="2" t="s">
+        <v>897</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A56" s="5" t="s">
+        <v>898</v>
+      </c>
+      <c r="B56" s="17" t="s">
+        <v>899</v>
+      </c>
+      <c r="C56" s="17" t="s">
+        <v>900</v>
+      </c>
+      <c r="D56" s="17" t="s">
+        <v>689</v>
+      </c>
+      <c r="E56" s="17" t="s">
+        <v>901</v>
+      </c>
+      <c r="F56" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G56" s="2" t="s">
+        <v>902</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A57" s="5" t="s">
+        <v>903</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>904</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>905</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>906</v>
+      </c>
+      <c r="E57" s="19" t="s">
+        <v>907</v>
+      </c>
+      <c r="F57" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>908</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+      <c r="A58" s="16" t="s">
+        <v>909</v>
+      </c>
+      <c r="B58" s="19" t="s">
+        <v>688</v>
+      </c>
+      <c r="C58" s="19" t="s">
+        <v>910</v>
+      </c>
+      <c r="D58" s="19" t="s">
+        <v>911</v>
+      </c>
+      <c r="E58" s="19" t="s">
+        <v>912</v>
+      </c>
+      <c r="F58" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>913</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="75" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>914</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>915</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>916</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>696</v>
+      </c>
+      <c r="E59" s="5" t="s">
+        <v>917</v>
+      </c>
+      <c r="F59" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>918</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68.5703125" customWidth="1"/>
+    <col min="7" max="7" width="109.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="16"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="19"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="16"/>
+      <c r="B3" s="19"/>
+      <c r="C3" s="19"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="11"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>